<commit_message>
modified:   output/chunk_3_18-02-2024.xlsx 	modified:   user_counter.json
</commit_message>
<xml_diff>
--- a/output/chunk_3_18-02-2024.xlsx
+++ b/output/chunk_3_18-02-2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Z28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2346,20 +2346,16 @@
           <t>XR3Z 10890 AA</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>191721894298</t>
-        </is>
+      <c r="C23" t="n">
+        <v>191721894298</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
           <t>['https://i.ebayimg.com/00/s/MTAwMFgxMDAw/z/Ca0AAOSw9mpaNAa7/$_1.JPG?set_id=8800005007']</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>262192</t>
-        </is>
+      <c r="E23" t="n">
+        <v>262192</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -2422,24 +2418,462 @@
           <t>1999</t>
         </is>
       </c>
-      <c r="W23" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="W23" t="n">
+        <v>60</v>
       </c>
       <c r="X23" t="inlineStr">
         <is>
           <t>OEM NEW Dashboard Instrument Panel Gauge Cluster Cover Mustang XR3Z-10890-AA</t>
         </is>
       </c>
-      <c r="Y23" t="inlineStr">
-        <is>
-          <t>38.88</t>
-        </is>
+      <c r="Y23" t="n">
+        <v>38.88</v>
       </c>
       <c r="Z23" t="inlineStr">
         <is>
           <t>[{'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.9L 238Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.9L 238Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Mach 1 Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Mach 1 Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra 10th Anniversary Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra 10th Anniversary Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Bullitt Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra R Coupe 2-Door', 'Engine': '5.4L 330Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>XR3Z 13008 AA</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>285536688931</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>['https://i.ebayimg.com/00/s/MzExWDEwMDA=/z/kEgAAOSw1T1itGp9/$_12.JPG?set_id=880000500F']</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>33710</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>eBay Motors:Parts &amp; Accessories:Car &amp; Truck Parts &amp; Accessories:Lighting &amp; Lamps:Headlight Assemblies</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>XR3Z13008AA,</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>1590269</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Mustang</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>Dorman</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>Headlight Lens</t>
+        </is>
+      </c>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>1999</t>
+        </is>
+      </c>
+      <c r="W24" t="n">
+        <v>19</v>
+      </c>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>FITS 1999-2000 FORD MUSTANG PASSENGER RIGHT FRONT HEADLIGHT LAMP ASSEMBLY</t>
+        </is>
+      </c>
+      <c r="Y24" t="n">
+        <v>70.58</v>
+      </c>
+      <c r="Z24" t="inlineStr">
+        <is>
+          <t>[{'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra R Coupe 2-Door', 'Engine': '5.4L 330Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>XR3Z 13008 BA</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>225489030756</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>['https://i.ebayimg.com/00/s/MTIwMFgxNjAw/z/POMAAOSwTMFkBhIq/$_12.JPG?set_id=880000500F']</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>33710</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>eBay Motors:Parts &amp; Accessories:Car &amp; Truck Parts &amp; Accessories:Lighting &amp; Lamps:Headlight Assemblies</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>1999 2000 2001 2002 2003 2004 Mustang Ford 114-640AL 20-5696-01</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>1999 2000 2001 2002 2003 2004 Mustang Ford 114-640AL 20-5696-01</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>LHT01364</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>1ALHL00369</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>DNA Motoring</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>['Front']</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>Headlight Assembly</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
+      <c r="X25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Driver Side  NEW for 99-04 Mustang  LED Headlight </t>
+        </is>
+      </c>
+      <c r="Y25" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>XR3Z 13405 AA</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>186118606968</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>['https://i.ebayimg.com/00/s/MTAzOFgxNDE3/z/FYIAAOSwWe1lKBk1/$_57.PNG?set_id=880000500F']</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>33716</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>eBay Motors:Parts &amp; Accessories:Car &amp; Truck Parts &amp; Accessories:Lighting &amp; Lamps:Tail Light Assemblies</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>XR3Z13405AA,YR3Z13405AA</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>XR3Z13405AA,YR3Z13405AA</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Mustang</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>['GT, LH']</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>Tail Light Assembly</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>1999</t>
+        </is>
+      </c>
+      <c r="W26" t="n">
+        <v>64</v>
+      </c>
+      <c r="X26" t="inlineStr">
+        <is>
+          <t>2000 Ford Mustang Gt Driver Left Tail Light Lamp Assembly Outer 99 01 02 03 04</t>
+        </is>
+      </c>
+      <c r="Y26" t="n">
+        <v>69.98999999999999</v>
+      </c>
+      <c r="Z26" t="inlineStr">
+        <is>
+          <t>[{'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.9L 238Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.9L 238Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Mach 1 Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Mach 1 Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra 10th Anniversary Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra 10th Anniversary Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Bullitt Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra R Coupe 2-Door', 'Engine': '5.4L 330Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>XR3Z 13550 AA</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>193020772458</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>['https://i.ebayimg.com/00/s/MTAwMFgxMDAw/z/iiUAAOSwdW9lvaXn/$_1.JPG?set_id=880000500F']</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>262208</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>eBay Motors:Parts &amp; Accessories:Car &amp; Truck Parts &amp; Accessories:Lighting &amp; Lamps:License Plate Light Assemblies</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2004 2003 2002 2001 2000 1999 1998 1997 1996 1995</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>F4ZZ13550A</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>2004 2003 2002 2001 2000 1999 1998 1997 1996 1995</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>OEM#B2894G0B2899G_94_95_96_97_98_99_00_01_02_03_N4</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Mustang</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>Venom Inc.</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>['Rear']</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>License Plate Light Assembly</t>
+        </is>
+      </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>1994</t>
+        </is>
+      </c>
+      <c r="W27" t="n">
+        <v>113</v>
+      </c>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>[2PCs] OE-Style License Plate Light Lens Lamp Replacement For 94-04 Ford Mustang</t>
+        </is>
+      </c>
+      <c r="Y27" t="n">
+        <v>11.83</v>
+      </c>
+      <c r="Z27" t="inlineStr">
+        <is>
+          <t>[{'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.9L 238Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.9L 238Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Mach 1 Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Mach 1 Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra 10th Anniversary Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra 10th Anniversary Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Bullitt Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra R Coupe 2-Door', 'Engine': '5.4L 330Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1998', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1998', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1998', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1998', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1998', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1998', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1998', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1998', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1998', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Semi-Equipado Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1998', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Semi-Equipado Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1998', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1998', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1997', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1997', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1997', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1997', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1997', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1997', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1997', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1997', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'High Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1997', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'High Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1997', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'High Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1997', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'High Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1997', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1997', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1996', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1996', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1996', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1996', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1996', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1996', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1996', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'High Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1996', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'High Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1996', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1996', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1995', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1995', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1995', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '5.0L 302Cu. In. V8 GAS OHV Naturally Aspirated'}, {'Year': '1995', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '5.0L 302Cu. In. V8 GAS OHV Naturally Aspirated'}, {'Year': '1995', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GTS Coupe 2-Door', 'Engine': '5.0L 302Cu. In. V8 GAS OHV Naturally Aspirated'}, {'Year': '1995', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '5.0L 302Cu. In. V8 GAS OHV Naturally Aspirated'}, {'Year': '1995', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '5.0L 302Cu. In. V8 GAS OHV Naturally Aspirated'}, {'Year': '1995', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra R Coupe 2-Door', 'Engine': '5.8L 5753CC 351Cu. In. V8 GAS OHV Naturally Aspirated'}, {'Year': '1994', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1994', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1994', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '5.0L 302Cu. In. V8 GAS OHV Naturally Aspirated'}, {'Year': '1994', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '5.0L 302Cu. In. V8 GAS OHV Naturally Aspirated'}, {'Year': '1994', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '5.0L 302Cu. In. V8 GAS OHV Naturally Aspirated'}, {'Year': '1994', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '5.0L 302Cu. In. V8 GAS OHV Naturally Aspirated'}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>XR3Z 15200 BA</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>304313415864</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>['https://i.ebayimg.com/00/s/MTUwMFgxNTAw/z/4yIAAOSwcn9hMc0j/$_1.JPG?set_id=880000500F']</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>33709</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>eBay Motors:Parts &amp; Accessories:Car &amp; Truck Parts &amp; Accessories:Lighting &amp; Lamps:Fog Light Assemblies</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>FO2593178 FO2592178</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>XR3Z 15200 BA XE3Z 15200 AA</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Mustang</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>Superbautoparts</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>['Front']</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>1999</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>Fit 1999-2004 Ford Mustang Fog Lights Driving Bumper Lamps GT V6 w/ Switch 99-04</t>
+        </is>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>27.98</t>
+        </is>
+      </c>
+      <c r="Z28" t="inlineStr">
+        <is>
+          <t>[{'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.9L 238Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.9L 238Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2004', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra 10th Anniversary Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra 10th Anniversary Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2003', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Supercharged'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2002', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Bullitt Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2001', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '2000', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra R Coupe 2-Door', 'Engine': '5.4L 330Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '3.8L 232Cu. In. V6 GAS OHV Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'Base Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'GT Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS SOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Convertible 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}, {'Year': '1999', 'Make': 'Ford', 'Model': 'Mustang', 'Trim': 'SVT Cobra Coupe 2-Door', 'Engine': '4.6L 281Cu. In. V8 GAS DOHC Naturally Aspirated'}]</t>
         </is>
       </c>
     </row>

</xml_diff>